<commit_message>
feat: adding new merge table in excel
</commit_message>
<xml_diff>
--- a/extract_list/outputs/amazonmx-suplementos.xlsx
+++ b/extract_list/outputs/amazonmx-suplementos.xlsx
@@ -1005,9 +1005,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="135.5703125" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>